<commit_message>
Added NPV, IRR and NP.
</commit_message>
<xml_diff>
--- a/balance_amzn.xlsx
+++ b/balance_amzn.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oienh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oienh\Documents\R_UNIVERSITY_PROJECTS\5th_Semester\trabajo_grupal_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B467F847-7319-4E79-8297-A84A14A65F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D1C6F1-FE23-435D-9753-0BFCB211C9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{65BF8A3D-7EE0-4BB6-B106-D71963C1F4F1}"/>
   </bookViews>
@@ -108,18 +108,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -446,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3364C4F4-D3A4-4718-AB7B-D4691AF39A2C}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -458,53 +457,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="5">
         <v>44926</v>
       </c>
-      <c r="C1" s="6">
+      <c r="C1" s="5">
         <v>44561</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1" s="5">
         <v>44196</v>
       </c>
-      <c r="E1" s="6">
+      <c r="E1" s="5">
         <v>43830</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>462675000</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>420549000</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>321195000</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>225248000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>462675000</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>420549000</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>321195000</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>225248000</v>
       </c>
     </row>
@@ -543,18 +542,6 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>